<commit_message>
modify the varibale name so that the program can be used by both chinese and english users
add english instructions and update the instructions to be more clear
</commit_message>
<xml_diff>
--- a/artifacts.xlsx
+++ b/artifacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\尹豪杰\Pictures\artifact_calculator_demo4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9228BF5F-CBF8-4166-B778-D4268EF7E553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C036FEA8-3F59-4585-9548-85A99B2B6583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="2775" windowWidth="16200" windowHeight="9360" xr2:uid="{4709D396-3847-41DC-A145-7953497538F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{4709D396-3847-41DC-A145-7953497538F4}"/>
   </bookViews>
   <sheets>
     <sheet name="artifacts" sheetId="1" r:id="rId1"/>
@@ -86,9 +86,6 @@
     <t>def=16</t>
   </si>
   <si>
-    <t>杯</t>
-  </si>
-  <si>
     <t>crit_dmg=6.2%</t>
   </si>
   <si>
@@ -98,18 +95,12 @@
     <t>crit_dmg=14.8%</t>
   </si>
   <si>
-    <t>沙</t>
-  </si>
-  <si>
     <t>hp=448</t>
   </si>
   <si>
     <t>def=19</t>
   </si>
   <si>
-    <t>羽</t>
-  </si>
-  <si>
     <t>crit_rate=5.8%</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>hp=11.1%</t>
   </si>
   <si>
-    <t>花</t>
-  </si>
-  <si>
     <t>hp=4780</t>
   </si>
   <si>
@@ -137,9 +125,6 @@
     <t>crit_rate=3.1%</t>
   </si>
   <si>
-    <t>冠</t>
-  </si>
-  <si>
     <t>crit_rate=31.1%</t>
   </si>
   <si>
@@ -336,6 +321,21 @@
   </si>
   <si>
     <t>set_number</t>
+  </si>
+  <si>
+    <t>goblet</t>
+  </si>
+  <si>
+    <t>sands</t>
+  </si>
+  <si>
+    <t>plume</t>
+  </si>
+  <si>
+    <t>flower</t>
+  </si>
+  <si>
+    <t>circlect</t>
   </si>
 </sst>
 </file>
@@ -713,7 +713,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +727,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -747,508 +747,508 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B2">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B4">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B5">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B6">
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B7">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B8">
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B9">
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B10">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B11">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="B12">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="B13">
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="B16">
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="B17">
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="B18">
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="B19">
         <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>89</v>
       </c>
       <c r="B20">
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
         <v>47</v>
       </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" t="s">
-        <v>52</v>
-      </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="B21">
         <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G21" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="B22">
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="B23">
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F23" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>